<commit_message>
added more fields for transaction evaluation
</commit_message>
<xml_diff>
--- a/data/UseCaseWeighting/datasets_5_15/UCP_DatasetV2.9.1.xlsx
+++ b/data/UseCaseWeighting/datasets_5_15/UCP_DatasetV2.9.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flyqk\Documents\Google Drive\ResearchSpace\Research Projects\UMLx\data\UseCaseWeighting\datasets_4_29\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flyqk\Documents\Google Drive\ResearchSpace\Research Projects\UMLx\data\UseCaseWeighting\datasets_5_15\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="UCP_DatasetV2.9.1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 

</xml_diff>